<commit_message>
remove error in identify in model
</commit_message>
<xml_diff>
--- a/reports.xlsx
+++ b/reports.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -378,22 +378,10 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>160130107024</t>
+          <t>160130107082</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
-        <is>
-          <t>Jaymin Patel</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>160130107082</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
         <is>
           <t>Umang Patel</t>
         </is>

</xml_diff>

<commit_message>
for checkout pull request from db
</commit_message>
<xml_diff>
--- a/reports.xlsx
+++ b/reports.xlsx
@@ -1,17 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
-  <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Cse15" sheetId="1" state="visible" r:id="rId1"/>
-  </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr codeName="ThisWorkbook"/>
+  <s:bookViews>
+    <s:workbookView activeTab="0"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="Cse15" sheetId="1" r:id="rId1"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
+</s:workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+  <si>
+    <t>Roll Number</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>03_05_20</t>
+  </si>
+  <si>
+    <t>04_05_20</t>
+  </si>
+  <si>
+    <t>160130107082</t>
+  </si>
+  <si>
+    <t>Umang Patel</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -47,11 +69,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -345,46 +368,38 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Roll Number</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>03_05_20</t>
-        </is>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>160130107082</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Umang Patel</t>
-        </is>
+    <row r="2" spans="1:4"/>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>